<commit_message>
konecna verzia, dodatocne upravy
</commit_message>
<xml_diff>
--- a/tabulka.xlsx
+++ b/tabulka.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubom\Desktop\stu\MIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubom\Desktop\stu\MIP\gitdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AAB7EBF-7DE3-45A3-90E3-6F786927B2DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B23D7B-D412-4963-8900-28C2FCF3D3D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="6300" xr2:uid="{DC14708B-2B89-4394-994F-104B2BFE000B}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Integračné a systémové testovanie</t>
   </si>
   <si>
-    <t>testovanie zákazníkom a Beta testy</t>
-  </si>
-  <si>
     <t>Vyexpedovaný produkt</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>zhromaždovanie požiadaviek, analýza a návrh</t>
+  </si>
+  <si>
+    <t>Testovanie zákazníkom a Beta testy</t>
   </si>
 </sst>
 </file>
@@ -429,87 +429,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD943736-4ADD-4EF6-9BC1-AA7482882B6B}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,132 +845,132 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7">
         <v>3.5</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="8">
         <v>10.5</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="8">
         <v>35</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="8">
         <v>6</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="9">
         <v>15</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="10">
         <f>SUM(C4:G4)</f>
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13">
         <v>6</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="13">
         <v>9</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="13">
         <v>2</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="14">
         <v>3</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="23">
         <f>SUM(C5:G5)</f>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17">
         <v>6.5</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="17">
         <v>1</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="18">
         <v>2.5</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="19">
         <f>SUM(C6:G6)</f>
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="25">
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20">
         <f>SUM(C4:C6)</f>
         <v>3.5</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <f>SUM(D4:D6)</f>
         <v>16.5</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="21">
         <f>SUM(E4:E6)</f>
         <v>50.5</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="21">
         <f>SUM(F4:F6)</f>
         <v>9</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="22">
         <f>SUM(G4:G6)</f>
         <v>20.5</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="24">
         <f>SUM(H4:H6)/100</f>
         <v>1</v>
       </c>

</xml_diff>